<commit_message>
Hexlet progress update of 25/05
</commit_message>
<xml_diff>
--- a/Before3.xlsx
+++ b/Before3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="125">
   <si>
     <t>JS: Обработка ошибок</t>
   </si>
@@ -321,6 +321,75 @@
   </si>
   <si>
     <t>Всякие селекторы типа puk[bduk] HTTP не понимает, это все надо распарсивать самому</t>
+  </si>
+  <si>
+    <t>Transfer-Encoding: chunked</t>
+  </si>
+  <si>
+    <t>Строка запроса имеет ограниченную длину</t>
+  </si>
+  <si>
+    <t>В POST тоже можно передавать строку запроса, причем вместе с body</t>
+  </si>
+  <si>
+    <t>GET идемпотентен, система не меняется</t>
+  </si>
+  <si>
+    <t>POST предназначен для изменения данных. Второй ПОСТ может привести к другому ответу и другим модификациям.</t>
+  </si>
+  <si>
+    <t>ПОСТы никогда не кэшируются</t>
+  </si>
+  <si>
+    <t>Формы бывают: - на создание и - на выборку.</t>
+  </si>
+  <si>
+    <t>на создание отправляется ПОСТ, на выборку - ГЕТ</t>
+  </si>
+  <si>
+    <t>301 Permanently используется например для перевода с http на https</t>
+  </si>
+  <si>
+    <t>Поисковики не выкидывают из индекса такие страницы</t>
+  </si>
+  <si>
+    <t>Куды идти указано в заголовке location</t>
+  </si>
+  <si>
+    <t>Команду printf 'Aladdin:open sesame' | base64 надо, блядь, с кавычками выполнять</t>
+  </si>
+  <si>
+    <t>Authorization: Basic &lt;base64 encoded login:password&gt;</t>
+  </si>
+  <si>
+    <t>HTTP - stateless protocol. Где тогда чо хранить?</t>
+  </si>
+  <si>
+    <t>В curl тоже есть флаги типа --head</t>
+  </si>
+  <si>
+    <t>Каждая кука посылается отдельно через свой Set-cookie:</t>
+  </si>
+  <si>
+    <t>Кука - это хрень ключ=значение; доп_параметры</t>
+  </si>
+  <si>
+    <t>Куки бывают сессионные и персистентные</t>
+  </si>
+  <si>
+    <t>domain, path, max-age, expires</t>
+  </si>
+  <si>
+    <t>Удаление куки: послать max-age равный НУЛЮ</t>
+  </si>
+  <si>
+    <t>HttpOnly - кука не будет отправлена жабаскриптом или аяксом</t>
+  </si>
+  <si>
+    <t>Отправка кук: Cookie: key=value; key1=value1</t>
+  </si>
+  <si>
+    <t>Параметры кук не отправляются</t>
   </si>
 </sst>
 </file>
@@ -687,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,40 +869,40 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13">
-        <v>1</v>
+      <c r="D13" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14">
-        <v>1</v>
+      <c r="D14" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D15">
-        <v>1</v>
+      <c r="D15" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
-        <v>1</v>
+      <c r="D16" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17">
-        <v>1</v>
+      <c r="D17" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1083,7 +1152,7 @@
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D48">
         <f>SUM(D2:D46)</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E48">
         <f>SUM(E2:E46)</f>
@@ -1096,7 +1165,7 @@
       </c>
       <c r="C50" s="1">
         <f ca="1">TODAY()</f>
-        <v>43244</v>
+        <v>43245</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
@@ -1113,7 +1182,7 @@
       </c>
       <c r="C52" s="2">
         <f ca="1">_xlfn.DAYS(C51,C50)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
@@ -1122,7 +1191,7 @@
       </c>
       <c r="C53">
         <f>D48+E48</f>
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
@@ -1131,7 +1200,7 @@
       </c>
       <c r="C54" s="5">
         <f ca="1">C53/C52</f>
-        <v>1.5</v>
+        <v>1.2941176470588236</v>
       </c>
     </row>
   </sheetData>
@@ -1142,15 +1211,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C45"/>
+  <dimension ref="B3:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
@@ -1387,6 +1456,136 @@
         <v>101</v>
       </c>
     </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>